<commit_message>
Add - Modelo BD E-R
</commit_message>
<xml_diff>
--- a/Versionado de Documentos/Modelo Actividades/Diagramas - Devs_lutions (v.4.0).xlsx
+++ b/Versionado de Documentos/Modelo Actividades/Diagramas - Devs_lutions (v.4.0).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alegv\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alegv\Documents\Escuela\Administración de Proyectos de Software\App\Devs_lutions\Versionado de Documentos\Modelo Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814D5DBE-DE0B-4AF0-B85B-D6A6A02C8512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070B6D5A-3A0F-4253-9F8E-6B3B92862A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="168">
   <si>
     <t>Actividades Clave</t>
   </si>
@@ -527,13 +527,19 @@
     <t>Meses de Trabajo</t>
   </si>
   <si>
-    <t>Personas / Mes</t>
-  </si>
-  <si>
     <t>Personas en el equipo de Desarrollo (Equipo)</t>
   </si>
   <si>
     <t>Horas por Persona</t>
+  </si>
+  <si>
+    <t>Horas /Persona</t>
+  </si>
+  <si>
+    <t>Mes / Personas</t>
+  </si>
+  <si>
+    <t>20 Días Disponibles en el Mes</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1715,6 +1721,22 @@
     <xf numFmtId="0" fontId="17" fillId="29" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1745,46 +1767,61 @@
     <xf numFmtId="0" fontId="3" fillId="24" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="43" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="43" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="39" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="42" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="41" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1811,25 +1848,37 @@
     <xf numFmtId="0" fontId="21" fillId="40" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="42" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="39" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="43" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="43" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="29" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1841,67 +1890,36 @@
     <xf numFmtId="0" fontId="29" fillId="29" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -40848,7 +40866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -40862,61 +40882,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
-      <c r="M1" s="131"/>
-      <c r="N1" s="131"/>
-      <c r="O1" s="132"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="137"/>
+      <c r="O1" s="138"/>
       <c r="P1" s="67"/>
     </row>
     <row r="2" spans="1:16" ht="27" customHeight="1">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="132" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="139" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="135" t="s">
+      <c r="C2" s="140"/>
+      <c r="D2" s="141" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="136"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="135" t="s">
+      <c r="E2" s="142"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="141" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="135" t="s">
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="141" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="136"/>
-      <c r="M2" s="136"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="137" t="s">
+      <c r="L2" s="142"/>
+      <c r="M2" s="142"/>
+      <c r="N2" s="140"/>
+      <c r="O2" s="143" t="s">
         <v>94</v>
       </c>
       <c r="P2" s="67"/>
     </row>
     <row r="3" spans="1:16" ht="27" customHeight="1">
-      <c r="A3" s="127"/>
-      <c r="B3" s="138" t="s">
+      <c r="A3" s="133"/>
+      <c r="B3" s="144" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="132"/>
+      <c r="C3" s="138"/>
       <c r="D3" s="68" t="s">
         <v>96</v>
       </c>
@@ -40950,11 +40970,11 @@
       <c r="N3" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="127"/>
+      <c r="O3" s="133"/>
       <c r="P3" s="67"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="134" t="s">
         <v>100</v>
       </c>
       <c r="B4" s="40">
@@ -40963,7 +40983,7 @@
       <c r="C4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="70"/>
+      <c r="D4" s="196"/>
       <c r="E4" s="71"/>
       <c r="F4" s="72"/>
       <c r="G4" s="72"/>
@@ -40982,7 +41002,7 @@
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="129"/>
+      <c r="A5" s="135"/>
       <c r="B5" s="40">
         <v>1.1000000000000001</v>
       </c>
@@ -41006,7 +41026,7 @@
       <c r="P5" s="67"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="129"/>
+      <c r="A6" s="135"/>
       <c r="B6" s="40">
         <v>1.2</v>
       </c>
@@ -41030,7 +41050,7 @@
       <c r="P6" s="67"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="129"/>
+      <c r="A7" s="135"/>
       <c r="B7" s="40">
         <v>1.3</v>
       </c>
@@ -41054,7 +41074,7 @@
       <c r="P7" s="67"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="129"/>
+      <c r="A8" s="135"/>
       <c r="B8" s="40">
         <v>2</v>
       </c>
@@ -41080,7 +41100,7 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="129"/>
+      <c r="A9" s="135"/>
       <c r="B9" s="40">
         <v>2.1</v>
       </c>
@@ -41104,7 +41124,7 @@
       <c r="P9" s="67"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="129"/>
+      <c r="A10" s="135"/>
       <c r="B10" s="40">
         <v>2.2000000000000002</v>
       </c>
@@ -41128,7 +41148,7 @@
       <c r="P10" s="67"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="129"/>
+      <c r="A11" s="135"/>
       <c r="B11" s="40">
         <v>2.2999999999999998</v>
       </c>
@@ -41152,7 +41172,7 @@
       <c r="P11" s="67"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="129"/>
+      <c r="A12" s="135"/>
       <c r="B12" s="40">
         <v>2.4</v>
       </c>
@@ -41176,7 +41196,7 @@
       <c r="P12" s="67"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="129"/>
+      <c r="A13" s="135"/>
       <c r="B13" s="40">
         <v>2.5</v>
       </c>
@@ -41200,7 +41220,7 @@
       <c r="P13" s="67"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="129"/>
+      <c r="A14" s="135"/>
       <c r="B14" s="40">
         <v>3</v>
       </c>
@@ -41226,7 +41246,7 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="129"/>
+      <c r="A15" s="135"/>
       <c r="B15" s="40">
         <v>3.1</v>
       </c>
@@ -41250,7 +41270,7 @@
       <c r="P15" s="67"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="129"/>
+      <c r="A16" s="135"/>
       <c r="B16" s="40">
         <v>3.2</v>
       </c>
@@ -41274,7 +41294,7 @@
       <c r="P16" s="67"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="129"/>
+      <c r="A17" s="135"/>
       <c r="B17" s="40">
         <v>4</v>
       </c>
@@ -41300,7 +41320,7 @@
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="129"/>
+      <c r="A18" s="135"/>
       <c r="B18" s="40">
         <v>4.0999999999999996</v>
       </c>
@@ -41324,7 +41344,7 @@
       <c r="P18" s="67"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="129"/>
+      <c r="A19" s="135"/>
       <c r="B19" s="40">
         <v>4.2</v>
       </c>
@@ -41348,7 +41368,7 @@
       <c r="P19" s="67"/>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="129"/>
+      <c r="A20" s="135"/>
       <c r="B20" s="40">
         <v>5</v>
       </c>
@@ -41374,7 +41394,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A21" s="129"/>
+      <c r="A21" s="135"/>
       <c r="B21" s="40">
         <v>5.0999999999999996</v>
       </c>
@@ -41398,7 +41418,7 @@
       <c r="P21" s="67"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A22" s="129"/>
+      <c r="A22" s="135"/>
       <c r="B22" s="40">
         <v>5.2</v>
       </c>
@@ -41422,7 +41442,7 @@
       <c r="P22" s="67"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A23" s="129"/>
+      <c r="A23" s="135"/>
       <c r="B23" s="40">
         <v>5.3</v>
       </c>
@@ -41446,7 +41466,7 @@
       <c r="P23" s="67"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A24" s="129"/>
+      <c r="A24" s="135"/>
       <c r="B24" s="40">
         <v>5.4</v>
       </c>
@@ -41470,7 +41490,7 @@
       <c r="P24" s="67"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A25" s="129"/>
+      <c r="A25" s="135"/>
       <c r="B25" s="40">
         <v>6</v>
       </c>
@@ -41496,7 +41516,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A26" s="129"/>
+      <c r="A26" s="135"/>
       <c r="B26" s="40">
         <v>6.1</v>
       </c>
@@ -41520,7 +41540,7 @@
       <c r="P26" s="67"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A27" s="129"/>
+      <c r="A27" s="135"/>
       <c r="B27" s="40">
         <v>6.2</v>
       </c>
@@ -41544,7 +41564,7 @@
       <c r="P27" s="67"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A28" s="129"/>
+      <c r="A28" s="135"/>
       <c r="B28" s="40">
         <v>6.3</v>
       </c>
@@ -41568,7 +41588,7 @@
       <c r="P28" s="67"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A29" s="129"/>
+      <c r="A29" s="135"/>
       <c r="B29" s="40">
         <v>6.4</v>
       </c>
@@ -41592,7 +41612,7 @@
       <c r="P29" s="67"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A30" s="129"/>
+      <c r="A30" s="135"/>
       <c r="B30" s="40">
         <v>6.5</v>
       </c>
@@ -41616,7 +41636,7 @@
       <c r="P30" s="67"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A31" s="129"/>
+      <c r="A31" s="135"/>
       <c r="B31" s="40">
         <v>7</v>
       </c>
@@ -41642,7 +41662,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A32" s="129"/>
+      <c r="A32" s="135"/>
       <c r="B32" s="40">
         <v>7.1</v>
       </c>
@@ -41666,7 +41686,7 @@
       <c r="P32" s="67"/>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A33" s="129"/>
+      <c r="A33" s="135"/>
       <c r="B33" s="40">
         <v>7.2</v>
       </c>
@@ -41690,7 +41710,7 @@
       <c r="P33" s="67"/>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A34" s="129"/>
+      <c r="A34" s="135"/>
       <c r="B34" s="40">
         <v>7.3</v>
       </c>
@@ -41714,7 +41734,7 @@
       <c r="P34" s="67"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A35" s="129"/>
+      <c r="A35" s="135"/>
       <c r="B35" s="40">
         <v>7.4</v>
       </c>
@@ -41738,7 +41758,7 @@
       <c r="P35" s="67"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A36" s="129"/>
+      <c r="A36" s="135"/>
       <c r="B36" s="40">
         <v>7.5</v>
       </c>
@@ -41762,7 +41782,7 @@
       <c r="P36" s="67"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A37" s="129"/>
+      <c r="A37" s="135"/>
       <c r="B37" s="40">
         <v>8</v>
       </c>
@@ -41788,7 +41808,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A38" s="129"/>
+      <c r="A38" s="135"/>
       <c r="B38" s="40">
         <v>8.1</v>
       </c>
@@ -41812,7 +41832,7 @@
       <c r="P38" s="67"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A39" s="129"/>
+      <c r="A39" s="135"/>
       <c r="B39" s="40">
         <v>8.1999999999999993</v>
       </c>
@@ -41836,7 +41856,7 @@
       <c r="P39" s="67"/>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A40" s="129"/>
+      <c r="A40" s="135"/>
       <c r="B40" s="40">
         <v>8.3000000000000007</v>
       </c>
@@ -41860,7 +41880,7 @@
       <c r="P40" s="67"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A41" s="129"/>
+      <c r="A41" s="135"/>
       <c r="B41" s="40">
         <v>9</v>
       </c>
@@ -41886,7 +41906,7 @@
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A42" s="129"/>
+      <c r="A42" s="135"/>
       <c r="B42" s="40">
         <v>9.1</v>
       </c>
@@ -41910,7 +41930,7 @@
       <c r="P42" s="67"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A43" s="129"/>
+      <c r="A43" s="135"/>
       <c r="B43" s="40">
         <v>9.1999999999999993</v>
       </c>
@@ -41934,7 +41954,7 @@
       <c r="P43" s="67"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A44" s="129"/>
+      <c r="A44" s="135"/>
       <c r="B44" s="40">
         <v>9.3000000000000007</v>
       </c>
@@ -41958,7 +41978,7 @@
       <c r="P44" s="67"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A45" s="129"/>
+      <c r="A45" s="135"/>
       <c r="B45" s="40">
         <v>10</v>
       </c>
@@ -41984,7 +42004,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A46" s="129"/>
+      <c r="A46" s="135"/>
       <c r="B46" s="40">
         <v>11</v>
       </c>
@@ -42010,7 +42030,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A47" s="129"/>
+      <c r="A47" s="135"/>
       <c r="B47" s="40">
         <v>11.1</v>
       </c>
@@ -42034,7 +42054,7 @@
       <c r="P47" s="67"/>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A48" s="129"/>
+      <c r="A48" s="135"/>
       <c r="B48" s="40">
         <v>12</v>
       </c>
@@ -42060,7 +42080,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A49" s="129"/>
+      <c r="A49" s="135"/>
       <c r="B49" s="40">
         <v>12.1</v>
       </c>
@@ -42084,7 +42104,7 @@
       <c r="P49" s="67"/>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A50" s="129"/>
+      <c r="A50" s="135"/>
       <c r="B50" s="40">
         <v>12.2</v>
       </c>
@@ -42108,7 +42128,7 @@
       <c r="P50" s="67"/>
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A51" s="129"/>
+      <c r="A51" s="135"/>
       <c r="B51" s="40">
         <v>13</v>
       </c>
@@ -42132,7 +42152,7 @@
       <c r="P51" s="67"/>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A52" s="129"/>
+      <c r="A52" s="135"/>
       <c r="B52" s="40">
         <v>13.1</v>
       </c>
@@ -42156,7 +42176,7 @@
       <c r="P52" s="67"/>
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A53" s="129"/>
+      <c r="A53" s="135"/>
       <c r="B53" s="40">
         <v>13.2</v>
       </c>
@@ -42180,7 +42200,7 @@
       <c r="P53" s="67"/>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A54" s="127"/>
+      <c r="A54" s="133"/>
       <c r="B54" s="40">
         <v>13.3</v>
       </c>
@@ -43182,7 +43202,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -43565,11 +43585,11 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="139" t="s">
+      <c r="A17" s="145" t="s">
         <v>114</v>
       </c>
-      <c r="B17" s="131"/>
-      <c r="C17" s="132"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="138"/>
       <c r="D17" s="101">
         <v>97</v>
       </c>
@@ -43591,8 +43611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26EABB90-BC04-47D3-BE5C-E7572BF784CD}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -43611,28 +43631,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="118" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="189" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="141" t="s">
+      <c r="B1" s="189"/>
+      <c r="C1" s="178" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="143"/>
-      <c r="L1" s="140" t="s">
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="179"/>
+      <c r="H1" s="179"/>
+      <c r="I1" s="179"/>
+      <c r="J1" s="179"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="177" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="104" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="149"/>
-      <c r="B2" s="149"/>
+      <c r="A2" s="189"/>
+      <c r="B2" s="189"/>
       <c r="C2" s="106" t="s">
         <v>129</v>
       </c>
@@ -43660,34 +43680,34 @@
       <c r="K2" s="111" t="s">
         <v>105</v>
       </c>
-      <c r="L2" s="140"/>
-      <c r="N2" s="154" t="s">
+      <c r="L2" s="177"/>
+      <c r="N2" s="165" t="s">
         <v>149</v>
       </c>
-      <c r="O2" s="155"/>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="156"/>
-      <c r="R2" s="154" t="s">
+      <c r="O2" s="166"/>
+      <c r="P2" s="166"/>
+      <c r="Q2" s="167"/>
+      <c r="R2" s="165" t="s">
         <v>150</v>
       </c>
-      <c r="S2" s="155"/>
-      <c r="T2" s="155"/>
-      <c r="U2" s="156"/>
-      <c r="V2" s="154" t="s">
+      <c r="S2" s="166"/>
+      <c r="T2" s="166"/>
+      <c r="U2" s="167"/>
+      <c r="V2" s="165" t="s">
         <v>151</v>
       </c>
-      <c r="W2" s="155"/>
-      <c r="X2" s="155"/>
-      <c r="Y2" s="156"/>
+      <c r="W2" s="166"/>
+      <c r="X2" s="166"/>
+      <c r="Y2" s="167"/>
     </row>
     <row r="3" spans="1:25" ht="42" customHeight="1">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="188" t="s">
         <v>121</v>
       </c>
       <c r="B3" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="165">
+      <c r="C3" s="127">
         <v>0</v>
       </c>
       <c r="D3" s="117">
@@ -43697,7 +43717,7 @@
         <f>C3*D3</f>
         <v>0</v>
       </c>
-      <c r="F3" s="165">
+      <c r="F3" s="127">
         <v>10</v>
       </c>
       <c r="G3" s="116">
@@ -43707,7 +43727,7 @@
         <f>G3*F3</f>
         <v>40</v>
       </c>
-      <c r="I3" s="165">
+      <c r="I3" s="127">
         <v>3</v>
       </c>
       <c r="J3" s="115">
@@ -43721,37 +43741,37 @@
         <f>K3+H3+E3</f>
         <v>58</v>
       </c>
-      <c r="N3" s="157" t="s">
+      <c r="N3" s="168" t="s">
         <v>152</v>
       </c>
-      <c r="O3" s="159" t="s">
+      <c r="O3" s="170" t="s">
         <v>148</v>
       </c>
-      <c r="P3" s="160"/>
-      <c r="Q3" s="161"/>
-      <c r="R3" s="157" t="s">
+      <c r="P3" s="171"/>
+      <c r="Q3" s="172"/>
+      <c r="R3" s="168" t="s">
         <v>153</v>
       </c>
-      <c r="S3" s="159" t="s">
+      <c r="S3" s="170" t="s">
         <v>148</v>
       </c>
-      <c r="T3" s="160"/>
-      <c r="U3" s="161"/>
-      <c r="V3" s="157" t="s">
+      <c r="T3" s="171"/>
+      <c r="U3" s="172"/>
+      <c r="V3" s="168" t="s">
         <v>153</v>
       </c>
-      <c r="W3" s="159" t="s">
+      <c r="W3" s="170" t="s">
         <v>148</v>
       </c>
-      <c r="X3" s="160"/>
-      <c r="Y3" s="161"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="172"/>
     </row>
     <row r="4" spans="1:25" ht="42" customHeight="1">
-      <c r="A4" s="147"/>
+      <c r="A4" s="187"/>
       <c r="B4" s="119" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="165">
+      <c r="C4" s="127">
         <v>6</v>
       </c>
       <c r="D4" s="117">
@@ -43761,7 +43781,7 @@
         <f t="shared" ref="E4:E6" si="0">C4*D4</f>
         <v>24</v>
       </c>
-      <c r="F4" s="165">
+      <c r="F4" s="127">
         <v>0</v>
       </c>
       <c r="G4" s="116">
@@ -43771,7 +43791,7 @@
         <f t="shared" ref="H4:H7" si="1">G4*F4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="165">
+      <c r="I4" s="127">
         <v>2</v>
       </c>
       <c r="J4" s="115">
@@ -43785,25 +43805,25 @@
         <f t="shared" ref="L4:L6" si="3">K4+H4+E4</f>
         <v>38</v>
       </c>
-      <c r="N4" s="158"/>
+      <c r="N4" s="169"/>
       <c r="O4" s="105"/>
       <c r="P4" s="105"/>
       <c r="Q4" s="105"/>
-      <c r="R4" s="158"/>
+      <c r="R4" s="169"/>
       <c r="S4" s="105"/>
       <c r="T4" s="105"/>
       <c r="U4" s="105"/>
-      <c r="V4" s="158"/>
+      <c r="V4" s="169"/>
       <c r="W4" s="105"/>
       <c r="X4" s="105"/>
       <c r="Y4" s="105"/>
     </row>
     <row r="5" spans="1:25" ht="42" customHeight="1">
-      <c r="A5" s="147"/>
+      <c r="A5" s="187"/>
       <c r="B5" s="119" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="165">
+      <c r="C5" s="127">
         <v>0</v>
       </c>
       <c r="D5" s="117">
@@ -43813,7 +43833,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" s="165">
+      <c r="F5" s="127">
         <v>12</v>
       </c>
       <c r="G5" s="116">
@@ -43823,7 +43843,7 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I5" s="165">
+      <c r="I5" s="127">
         <v>4</v>
       </c>
       <c r="J5" s="115">
@@ -43869,13 +43889,13 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="55.5" customHeight="1">
-      <c r="A6" s="147" t="s">
+      <c r="A6" s="187" t="s">
         <v>120</v>
       </c>
       <c r="B6" s="119" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="165">
+      <c r="C6" s="127">
         <v>5</v>
       </c>
       <c r="D6" s="117">
@@ -43885,7 +43905,7 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="F6" s="165">
+      <c r="F6" s="127">
         <v>0</v>
       </c>
       <c r="G6" s="116">
@@ -43895,7 +43915,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6" s="165">
+      <c r="I6" s="127">
         <v>0</v>
       </c>
       <c r="J6" s="115">
@@ -43941,11 +43961,11 @@
       </c>
     </row>
     <row r="7" spans="1:25" ht="55.5" customHeight="1">
-      <c r="A7" s="147"/>
+      <c r="A7" s="187"/>
       <c r="B7" s="119" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="165">
+      <c r="C7" s="127">
         <v>1</v>
       </c>
       <c r="D7" s="117">
@@ -43955,7 +43975,7 @@
         <f>C7*D7</f>
         <v>5</v>
       </c>
-      <c r="F7" s="165">
+      <c r="F7" s="127">
         <v>0</v>
       </c>
       <c r="G7" s="116">
@@ -43965,7 +43985,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7" s="165">
+      <c r="I7" s="127">
         <v>0</v>
       </c>
       <c r="J7" s="115">
@@ -44011,19 +44031,19 @@
       </c>
     </row>
     <row r="8" spans="1:25" ht="28.5" customHeight="1">
-      <c r="A8" s="144" t="s">
+      <c r="A8" s="181" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="145"/>
-      <c r="C8" s="145"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="145"/>
-      <c r="F8" s="145"/>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="145"/>
-      <c r="K8" s="146"/>
+      <c r="B8" s="182"/>
+      <c r="C8" s="182"/>
+      <c r="D8" s="182"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="182"/>
+      <c r="J8" s="182"/>
+      <c r="K8" s="183"/>
       <c r="L8" s="122">
         <f>SUM(L3:L7)</f>
         <v>208</v>
@@ -44031,19 +44051,19 @@
     </row>
     <row r="9" spans="1:25" ht="9.75" customHeight="1"/>
     <row r="10" spans="1:25" ht="27.75" customHeight="1">
-      <c r="A10" s="149" t="s">
+      <c r="A10" s="189" t="s">
         <v>130</v>
       </c>
-      <c r="B10" s="149"/>
-      <c r="C10" s="149"/>
-      <c r="D10" s="149"/>
-      <c r="E10" s="149"/>
-      <c r="F10" s="149"/>
-      <c r="G10" s="149"/>
-      <c r="H10" s="149"/>
-      <c r="I10" s="149"/>
-      <c r="J10" s="149"/>
-      <c r="K10" s="149"/>
+      <c r="B10" s="189"/>
+      <c r="C10" s="189"/>
+      <c r="D10" s="189"/>
+      <c r="E10" s="189"/>
+      <c r="F10" s="189"/>
+      <c r="G10" s="189"/>
+      <c r="H10" s="189"/>
+      <c r="I10" s="189"/>
+      <c r="J10" s="189"/>
+      <c r="K10" s="189"/>
       <c r="L10" s="125" t="s">
         <v>145</v>
       </c>
@@ -44052,18 +44072,18 @@
       <c r="A11" s="120">
         <v>1</v>
       </c>
-      <c r="B11" s="150" t="s">
+      <c r="B11" s="173" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="150"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="150"/>
-      <c r="F11" s="150"/>
-      <c r="G11" s="150"/>
-      <c r="H11" s="150"/>
-      <c r="I11" s="150"/>
-      <c r="J11" s="150"/>
-      <c r="K11" s="150"/>
+      <c r="C11" s="173"/>
+      <c r="D11" s="173"/>
+      <c r="E11" s="173"/>
+      <c r="F11" s="173"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="173"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="173"/>
+      <c r="K11" s="173"/>
       <c r="L11" s="105">
         <v>5</v>
       </c>
@@ -44072,449 +44092,449 @@
       <c r="A12" s="121">
         <v>2</v>
       </c>
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="173" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="150"/>
-      <c r="D12" s="150"/>
-      <c r="E12" s="150"/>
-      <c r="F12" s="150"/>
-      <c r="G12" s="150"/>
-      <c r="H12" s="150"/>
-      <c r="I12" s="150"/>
-      <c r="J12" s="150"/>
-      <c r="K12" s="150"/>
+      <c r="C12" s="173"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="173"/>
+      <c r="F12" s="173"/>
+      <c r="G12" s="173"/>
+      <c r="H12" s="173"/>
+      <c r="I12" s="173"/>
+      <c r="J12" s="173"/>
+      <c r="K12" s="173"/>
       <c r="L12" s="105">
         <v>4</v>
       </c>
-      <c r="N12" s="163">
+      <c r="N12" s="164">
         <v>0</v>
       </c>
-      <c r="O12" s="162" t="s">
+      <c r="O12" s="163" t="s">
         <v>154</v>
       </c>
-      <c r="P12" s="162"/>
-      <c r="Q12" s="162"/>
-      <c r="R12" s="162"/>
-      <c r="S12" s="162"/>
-      <c r="T12" s="162"/>
-      <c r="U12" s="162"/>
-      <c r="V12" s="162"/>
-      <c r="W12" s="162"/>
-      <c r="X12" s="162"/>
-      <c r="Y12" s="162"/>
+      <c r="P12" s="163"/>
+      <c r="Q12" s="163"/>
+      <c r="R12" s="163"/>
+      <c r="S12" s="163"/>
+      <c r="T12" s="163"/>
+      <c r="U12" s="163"/>
+      <c r="V12" s="163"/>
+      <c r="W12" s="163"/>
+      <c r="X12" s="163"/>
+      <c r="Y12" s="163"/>
     </row>
     <row r="13" spans="1:25" ht="20.25" customHeight="1">
       <c r="A13" s="121">
         <v>3</v>
       </c>
-      <c r="B13" s="150" t="s">
+      <c r="B13" s="173" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="150"/>
-      <c r="D13" s="150"/>
-      <c r="E13" s="150"/>
-      <c r="F13" s="150"/>
-      <c r="G13" s="150"/>
-      <c r="H13" s="150"/>
-      <c r="I13" s="150"/>
-      <c r="J13" s="150"/>
-      <c r="K13" s="150"/>
+      <c r="C13" s="173"/>
+      <c r="D13" s="173"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="105">
         <v>4</v>
       </c>
-      <c r="N13" s="163"/>
-      <c r="O13" s="162"/>
-      <c r="P13" s="162"/>
-      <c r="Q13" s="162"/>
-      <c r="R13" s="162"/>
-      <c r="S13" s="162"/>
-      <c r="T13" s="162"/>
-      <c r="U13" s="162"/>
-      <c r="V13" s="162"/>
-      <c r="W13" s="162"/>
-      <c r="X13" s="162"/>
-      <c r="Y13" s="162"/>
+      <c r="N13" s="164"/>
+      <c r="O13" s="163"/>
+      <c r="P13" s="163"/>
+      <c r="Q13" s="163"/>
+      <c r="R13" s="163"/>
+      <c r="S13" s="163"/>
+      <c r="T13" s="163"/>
+      <c r="U13" s="163"/>
+      <c r="V13" s="163"/>
+      <c r="W13" s="163"/>
+      <c r="X13" s="163"/>
+      <c r="Y13" s="163"/>
     </row>
     <row r="14" spans="1:25" ht="20.25" customHeight="1">
       <c r="A14" s="121">
         <v>4</v>
       </c>
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="173" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="150"/>
-      <c r="D14" s="150"/>
-      <c r="E14" s="150"/>
-      <c r="F14" s="150"/>
-      <c r="G14" s="150"/>
-      <c r="H14" s="150"/>
-      <c r="I14" s="150"/>
-      <c r="J14" s="150"/>
-      <c r="K14" s="150"/>
+      <c r="C14" s="173"/>
+      <c r="D14" s="173"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="105">
         <v>2</v>
       </c>
-      <c r="N14" s="163">
+      <c r="N14" s="164">
         <v>1</v>
       </c>
-      <c r="O14" s="162" t="s">
+      <c r="O14" s="163" t="s">
         <v>155</v>
       </c>
-      <c r="P14" s="162"/>
-      <c r="Q14" s="162"/>
-      <c r="R14" s="162"/>
-      <c r="S14" s="162"/>
-      <c r="T14" s="162"/>
-      <c r="U14" s="162"/>
-      <c r="V14" s="162"/>
-      <c r="W14" s="162"/>
-      <c r="X14" s="162"/>
-      <c r="Y14" s="162"/>
+      <c r="P14" s="163"/>
+      <c r="Q14" s="163"/>
+      <c r="R14" s="163"/>
+      <c r="S14" s="163"/>
+      <c r="T14" s="163"/>
+      <c r="U14" s="163"/>
+      <c r="V14" s="163"/>
+      <c r="W14" s="163"/>
+      <c r="X14" s="163"/>
+      <c r="Y14" s="163"/>
     </row>
     <row r="15" spans="1:25" ht="20.25" customHeight="1">
       <c r="A15" s="121">
         <v>5</v>
       </c>
-      <c r="B15" s="150" t="s">
+      <c r="B15" s="173" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="150"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="150"/>
-      <c r="F15" s="150"/>
-      <c r="G15" s="150"/>
-      <c r="H15" s="150"/>
-      <c r="I15" s="150"/>
-      <c r="J15" s="150"/>
-      <c r="K15" s="150"/>
+      <c r="C15" s="173"/>
+      <c r="D15" s="173"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="105">
         <v>5</v>
       </c>
-      <c r="N15" s="163"/>
-      <c r="O15" s="162"/>
-      <c r="P15" s="162"/>
-      <c r="Q15" s="162"/>
-      <c r="R15" s="162"/>
-      <c r="S15" s="162"/>
-      <c r="T15" s="162"/>
-      <c r="U15" s="162"/>
-      <c r="V15" s="162"/>
-      <c r="W15" s="162"/>
-      <c r="X15" s="162"/>
-      <c r="Y15" s="162"/>
+      <c r="N15" s="164"/>
+      <c r="O15" s="163"/>
+      <c r="P15" s="163"/>
+      <c r="Q15" s="163"/>
+      <c r="R15" s="163"/>
+      <c r="S15" s="163"/>
+      <c r="T15" s="163"/>
+      <c r="U15" s="163"/>
+      <c r="V15" s="163"/>
+      <c r="W15" s="163"/>
+      <c r="X15" s="163"/>
+      <c r="Y15" s="163"/>
     </row>
     <row r="16" spans="1:25" ht="20.25" customHeight="1">
       <c r="A16" s="121">
         <v>6</v>
       </c>
-      <c r="B16" s="150" t="s">
+      <c r="B16" s="173" t="s">
         <v>136</v>
       </c>
-      <c r="C16" s="150"/>
-      <c r="D16" s="150"/>
-      <c r="E16" s="150"/>
-      <c r="F16" s="150"/>
-      <c r="G16" s="150"/>
-      <c r="H16" s="150"/>
-      <c r="I16" s="150"/>
-      <c r="J16" s="150"/>
-      <c r="K16" s="150"/>
+      <c r="C16" s="173"/>
+      <c r="D16" s="173"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="105">
         <v>5</v>
       </c>
-      <c r="N16" s="163">
+      <c r="N16" s="164">
         <v>2</v>
       </c>
-      <c r="O16" s="162" t="s">
+      <c r="O16" s="163" t="s">
         <v>156</v>
       </c>
-      <c r="P16" s="162"/>
-      <c r="Q16" s="162"/>
-      <c r="R16" s="162"/>
-      <c r="S16" s="162"/>
-      <c r="T16" s="162"/>
-      <c r="U16" s="162"/>
-      <c r="V16" s="162"/>
-      <c r="W16" s="162"/>
-      <c r="X16" s="162"/>
-      <c r="Y16" s="162"/>
+      <c r="P16" s="163"/>
+      <c r="Q16" s="163"/>
+      <c r="R16" s="163"/>
+      <c r="S16" s="163"/>
+      <c r="T16" s="163"/>
+      <c r="U16" s="163"/>
+      <c r="V16" s="163"/>
+      <c r="W16" s="163"/>
+      <c r="X16" s="163"/>
+      <c r="Y16" s="163"/>
     </row>
     <row r="17" spans="1:25" ht="20.25" customHeight="1">
       <c r="A17" s="121">
         <v>7</v>
       </c>
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="173" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="150"/>
-      <c r="D17" s="150"/>
-      <c r="E17" s="150"/>
-      <c r="F17" s="150"/>
-      <c r="G17" s="150"/>
-      <c r="H17" s="150"/>
-      <c r="I17" s="150"/>
-      <c r="J17" s="150"/>
-      <c r="K17" s="150"/>
+      <c r="C17" s="173"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="105">
         <v>3</v>
       </c>
-      <c r="N17" s="163"/>
-      <c r="O17" s="162"/>
-      <c r="P17" s="162"/>
-      <c r="Q17" s="162"/>
-      <c r="R17" s="162"/>
-      <c r="S17" s="162"/>
-      <c r="T17" s="162"/>
-      <c r="U17" s="162"/>
-      <c r="V17" s="162"/>
-      <c r="W17" s="162"/>
-      <c r="X17" s="162"/>
-      <c r="Y17" s="162"/>
+      <c r="N17" s="164"/>
+      <c r="O17" s="163"/>
+      <c r="P17" s="163"/>
+      <c r="Q17" s="163"/>
+      <c r="R17" s="163"/>
+      <c r="S17" s="163"/>
+      <c r="T17" s="163"/>
+      <c r="U17" s="163"/>
+      <c r="V17" s="163"/>
+      <c r="W17" s="163"/>
+      <c r="X17" s="163"/>
+      <c r="Y17" s="163"/>
     </row>
     <row r="18" spans="1:25" ht="20.25" customHeight="1">
       <c r="A18" s="121">
         <v>8</v>
       </c>
-      <c r="B18" s="150" t="s">
+      <c r="B18" s="173" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="150"/>
-      <c r="D18" s="150"/>
-      <c r="E18" s="150"/>
-      <c r="F18" s="150"/>
-      <c r="G18" s="150"/>
-      <c r="H18" s="150"/>
-      <c r="I18" s="150"/>
-      <c r="J18" s="150"/>
-      <c r="K18" s="150"/>
+      <c r="C18" s="173"/>
+      <c r="D18" s="173"/>
+      <c r="E18" s="173"/>
+      <c r="F18" s="173"/>
+      <c r="G18" s="173"/>
+      <c r="H18" s="173"/>
+      <c r="I18" s="173"/>
+      <c r="J18" s="173"/>
+      <c r="K18" s="173"/>
       <c r="L18" s="105">
         <v>2</v>
       </c>
-      <c r="N18" s="163">
+      <c r="N18" s="164">
         <v>3</v>
       </c>
-      <c r="O18" s="162" t="s">
+      <c r="O18" s="163" t="s">
         <v>157</v>
       </c>
-      <c r="P18" s="162"/>
-      <c r="Q18" s="162"/>
-      <c r="R18" s="162"/>
-      <c r="S18" s="162"/>
-      <c r="T18" s="162"/>
-      <c r="U18" s="162"/>
-      <c r="V18" s="162"/>
-      <c r="W18" s="162"/>
-      <c r="X18" s="162"/>
-      <c r="Y18" s="162"/>
+      <c r="P18" s="163"/>
+      <c r="Q18" s="163"/>
+      <c r="R18" s="163"/>
+      <c r="S18" s="163"/>
+      <c r="T18" s="163"/>
+      <c r="U18" s="163"/>
+      <c r="V18" s="163"/>
+      <c r="W18" s="163"/>
+      <c r="X18" s="163"/>
+      <c r="Y18" s="163"/>
     </row>
     <row r="19" spans="1:25" ht="20.25" customHeight="1">
       <c r="A19" s="121">
         <v>9</v>
       </c>
-      <c r="B19" s="150" t="s">
+      <c r="B19" s="173" t="s">
         <v>139</v>
       </c>
-      <c r="C19" s="150"/>
-      <c r="D19" s="150"/>
-      <c r="E19" s="150"/>
-      <c r="F19" s="150"/>
-      <c r="G19" s="150"/>
-      <c r="H19" s="150"/>
-      <c r="I19" s="150"/>
-      <c r="J19" s="150"/>
-      <c r="K19" s="150"/>
+      <c r="C19" s="173"/>
+      <c r="D19" s="173"/>
+      <c r="E19" s="173"/>
+      <c r="F19" s="173"/>
+      <c r="G19" s="173"/>
+      <c r="H19" s="173"/>
+      <c r="I19" s="173"/>
+      <c r="J19" s="173"/>
+      <c r="K19" s="173"/>
       <c r="L19" s="105">
         <v>1</v>
       </c>
-      <c r="N19" s="163"/>
-      <c r="O19" s="162"/>
-      <c r="P19" s="162"/>
-      <c r="Q19" s="162"/>
-      <c r="R19" s="162"/>
-      <c r="S19" s="162"/>
-      <c r="T19" s="162"/>
-      <c r="U19" s="162"/>
-      <c r="V19" s="162"/>
-      <c r="W19" s="162"/>
-      <c r="X19" s="162"/>
-      <c r="Y19" s="162"/>
+      <c r="N19" s="164"/>
+      <c r="O19" s="163"/>
+      <c r="P19" s="163"/>
+      <c r="Q19" s="163"/>
+      <c r="R19" s="163"/>
+      <c r="S19" s="163"/>
+      <c r="T19" s="163"/>
+      <c r="U19" s="163"/>
+      <c r="V19" s="163"/>
+      <c r="W19" s="163"/>
+      <c r="X19" s="163"/>
+      <c r="Y19" s="163"/>
     </row>
     <row r="20" spans="1:25" ht="20.25" customHeight="1">
       <c r="A20" s="121">
         <v>10</v>
       </c>
-      <c r="B20" s="150" t="s">
+      <c r="B20" s="173" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
-      <c r="H20" s="150"/>
-      <c r="I20" s="150"/>
-      <c r="J20" s="150"/>
-      <c r="K20" s="150"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="173"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="173"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173"/>
+      <c r="J20" s="173"/>
+      <c r="K20" s="173"/>
       <c r="L20" s="105">
         <v>3</v>
       </c>
-      <c r="N20" s="163">
+      <c r="N20" s="164">
         <v>4</v>
       </c>
-      <c r="O20" s="162" t="s">
+      <c r="O20" s="163" t="s">
         <v>158</v>
       </c>
-      <c r="P20" s="162"/>
-      <c r="Q20" s="162"/>
-      <c r="R20" s="162"/>
-      <c r="S20" s="162"/>
-      <c r="T20" s="162"/>
-      <c r="U20" s="162"/>
-      <c r="V20" s="162"/>
-      <c r="W20" s="162"/>
-      <c r="X20" s="162"/>
-      <c r="Y20" s="162"/>
+      <c r="P20" s="163"/>
+      <c r="Q20" s="163"/>
+      <c r="R20" s="163"/>
+      <c r="S20" s="163"/>
+      <c r="T20" s="163"/>
+      <c r="U20" s="163"/>
+      <c r="V20" s="163"/>
+      <c r="W20" s="163"/>
+      <c r="X20" s="163"/>
+      <c r="Y20" s="163"/>
     </row>
     <row r="21" spans="1:25" ht="20.25" customHeight="1">
       <c r="A21" s="121">
         <v>11</v>
       </c>
-      <c r="B21" s="150" t="s">
+      <c r="B21" s="173" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="150"/>
-      <c r="D21" s="150"/>
-      <c r="E21" s="150"/>
-      <c r="F21" s="150"/>
-      <c r="G21" s="150"/>
-      <c r="H21" s="150"/>
-      <c r="I21" s="150"/>
-      <c r="J21" s="150"/>
-      <c r="K21" s="150"/>
+      <c r="C21" s="173"/>
+      <c r="D21" s="173"/>
+      <c r="E21" s="173"/>
+      <c r="F21" s="173"/>
+      <c r="G21" s="173"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="173"/>
+      <c r="J21" s="173"/>
+      <c r="K21" s="173"/>
       <c r="L21" s="105">
         <v>3</v>
       </c>
-      <c r="N21" s="163"/>
-      <c r="O21" s="162"/>
-      <c r="P21" s="162"/>
-      <c r="Q21" s="162"/>
-      <c r="R21" s="162"/>
-      <c r="S21" s="162"/>
-      <c r="T21" s="162"/>
-      <c r="U21" s="162"/>
-      <c r="V21" s="162"/>
-      <c r="W21" s="162"/>
-      <c r="X21" s="162"/>
-      <c r="Y21" s="162"/>
+      <c r="N21" s="164"/>
+      <c r="O21" s="163"/>
+      <c r="P21" s="163"/>
+      <c r="Q21" s="163"/>
+      <c r="R21" s="163"/>
+      <c r="S21" s="163"/>
+      <c r="T21" s="163"/>
+      <c r="U21" s="163"/>
+      <c r="V21" s="163"/>
+      <c r="W21" s="163"/>
+      <c r="X21" s="163"/>
+      <c r="Y21" s="163"/>
     </row>
     <row r="22" spans="1:25" ht="20.25" customHeight="1">
       <c r="A22" s="121">
         <v>12</v>
       </c>
-      <c r="B22" s="150" t="s">
+      <c r="B22" s="173" t="s">
         <v>142</v>
       </c>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
-      <c r="H22" s="150"/>
-      <c r="I22" s="150"/>
-      <c r="J22" s="150"/>
-      <c r="K22" s="150"/>
+      <c r="C22" s="173"/>
+      <c r="D22" s="173"/>
+      <c r="E22" s="173"/>
+      <c r="F22" s="173"/>
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173"/>
+      <c r="J22" s="173"/>
+      <c r="K22" s="173"/>
       <c r="L22" s="105">
         <v>4</v>
       </c>
-      <c r="N22" s="163">
+      <c r="N22" s="164">
         <v>5</v>
       </c>
-      <c r="O22" s="162" t="s">
+      <c r="O22" s="163" t="s">
         <v>159</v>
       </c>
-      <c r="P22" s="162"/>
-      <c r="Q22" s="162"/>
-      <c r="R22" s="162"/>
-      <c r="S22" s="162"/>
-      <c r="T22" s="162"/>
-      <c r="U22" s="162"/>
-      <c r="V22" s="162"/>
-      <c r="W22" s="162"/>
-      <c r="X22" s="162"/>
-      <c r="Y22" s="162"/>
+      <c r="P22" s="163"/>
+      <c r="Q22" s="163"/>
+      <c r="R22" s="163"/>
+      <c r="S22" s="163"/>
+      <c r="T22" s="163"/>
+      <c r="U22" s="163"/>
+      <c r="V22" s="163"/>
+      <c r="W22" s="163"/>
+      <c r="X22" s="163"/>
+      <c r="Y22" s="163"/>
     </row>
     <row r="23" spans="1:25" ht="20.25" customHeight="1">
       <c r="A23" s="121">
         <v>13</v>
       </c>
-      <c r="B23" s="150" t="s">
+      <c r="B23" s="173" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="150"/>
-      <c r="D23" s="150"/>
-      <c r="E23" s="150"/>
-      <c r="F23" s="150"/>
-      <c r="G23" s="150"/>
-      <c r="H23" s="150"/>
-      <c r="I23" s="150"/>
-      <c r="J23" s="150"/>
-      <c r="K23" s="150"/>
+      <c r="C23" s="173"/>
+      <c r="D23" s="173"/>
+      <c r="E23" s="173"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="173"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="173"/>
+      <c r="J23" s="173"/>
+      <c r="K23" s="173"/>
       <c r="L23" s="105">
         <v>1</v>
       </c>
-      <c r="N23" s="163"/>
-      <c r="O23" s="162"/>
-      <c r="P23" s="162"/>
-      <c r="Q23" s="162"/>
-      <c r="R23" s="162"/>
-      <c r="S23" s="162"/>
-      <c r="T23" s="162"/>
-      <c r="U23" s="162"/>
-      <c r="V23" s="162"/>
-      <c r="W23" s="162"/>
-      <c r="X23" s="162"/>
-      <c r="Y23" s="162"/>
+      <c r="N23" s="164"/>
+      <c r="O23" s="163"/>
+      <c r="P23" s="163"/>
+      <c r="Q23" s="163"/>
+      <c r="R23" s="163"/>
+      <c r="S23" s="163"/>
+      <c r="T23" s="163"/>
+      <c r="U23" s="163"/>
+      <c r="V23" s="163"/>
+      <c r="W23" s="163"/>
+      <c r="X23" s="163"/>
+      <c r="Y23" s="163"/>
     </row>
     <row r="24" spans="1:25" ht="20.25" customHeight="1">
       <c r="A24" s="121">
         <v>14</v>
       </c>
-      <c r="B24" s="150" t="s">
+      <c r="B24" s="173" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="150"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="150"/>
-      <c r="F24" s="150"/>
-      <c r="G24" s="150"/>
-      <c r="H24" s="150"/>
-      <c r="I24" s="150"/>
-      <c r="J24" s="150"/>
-      <c r="K24" s="150"/>
+      <c r="C24" s="173"/>
+      <c r="D24" s="173"/>
+      <c r="E24" s="173"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="173"/>
+      <c r="H24" s="173"/>
+      <c r="I24" s="173"/>
+      <c r="J24" s="173"/>
+      <c r="K24" s="173"/>
       <c r="L24" s="105">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="84" customHeight="1">
-      <c r="A25" s="151"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="152" t="s">
+      <c r="A25" s="174"/>
+      <c r="B25" s="174"/>
+      <c r="C25" s="175" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="152"/>
-      <c r="E25" s="152"/>
-      <c r="F25" s="153">
+      <c r="D25" s="175"/>
+      <c r="E25" s="175"/>
+      <c r="F25" s="176">
         <f>(0.65 + (L25 * 0.01))</f>
         <v>1.0900000000000001</v>
       </c>
-      <c r="G25" s="153"/>
-      <c r="H25" s="153"/>
-      <c r="I25" s="152" t="s">
+      <c r="G25" s="176"/>
+      <c r="H25" s="176"/>
+      <c r="I25" s="175" t="s">
         <v>147</v>
       </c>
-      <c r="J25" s="152"/>
-      <c r="K25" s="152"/>
+      <c r="J25" s="175"/>
+      <c r="K25" s="175"/>
       <c r="L25" s="124">
         <f>SUM(L11:L24)</f>
         <v>44</v>
@@ -44522,208 +44542,174 @@
     </row>
     <row r="26" spans="1:25" ht="9.75" customHeight="1"/>
     <row r="27" spans="1:25" ht="31.5" customHeight="1">
-      <c r="A27" s="169" t="s">
+      <c r="A27" s="184" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="170"/>
-      <c r="C27" s="170"/>
-      <c r="D27" s="170"/>
-      <c r="E27" s="170"/>
-      <c r="F27" s="170"/>
-      <c r="G27" s="170"/>
-      <c r="H27" s="170"/>
-      <c r="I27" s="170"/>
-      <c r="J27" s="170"/>
-      <c r="K27" s="171"/>
+      <c r="B27" s="185"/>
+      <c r="C27" s="185"/>
+      <c r="D27" s="185"/>
+      <c r="E27" s="185"/>
+      <c r="F27" s="185"/>
+      <c r="G27" s="185"/>
+      <c r="H27" s="185"/>
+      <c r="I27" s="185"/>
+      <c r="J27" s="185"/>
+      <c r="K27" s="186"/>
       <c r="L27" s="122">
         <f>F25</f>
         <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="31.5" customHeight="1">
-      <c r="A28" s="169" t="s">
+      <c r="A28" s="184" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="170"/>
-      <c r="C28" s="170"/>
-      <c r="D28" s="170"/>
-      <c r="E28" s="170"/>
-      <c r="F28" s="170"/>
-      <c r="G28" s="170"/>
-      <c r="H28" s="170"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="170"/>
-      <c r="K28" s="171"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="185"/>
+      <c r="D28" s="185"/>
+      <c r="E28" s="185"/>
+      <c r="F28" s="185"/>
+      <c r="G28" s="185"/>
+      <c r="H28" s="185"/>
+      <c r="I28" s="185"/>
+      <c r="J28" s="185"/>
+      <c r="K28" s="186"/>
       <c r="L28" s="122">
         <f>L27*L8</f>
         <v>226.72000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="20.25">
-      <c r="A29" s="177"/>
+      <c r="A29" s="130"/>
     </row>
     <row r="30" spans="1:25" ht="31.5" customHeight="1">
-      <c r="A30" s="166" t="s">
+      <c r="A30" s="149" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="167"/>
-      <c r="C30" s="167"/>
-      <c r="D30" s="167"/>
-      <c r="E30" s="167"/>
-      <c r="F30" s="167"/>
-      <c r="G30" s="167"/>
-      <c r="H30" s="167"/>
-      <c r="I30" s="167"/>
-      <c r="J30" s="168"/>
-      <c r="K30" s="184" t="s">
+      <c r="B30" s="150"/>
+      <c r="C30" s="150"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="150"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="150"/>
+      <c r="H30" s="150"/>
+      <c r="I30" s="150"/>
+      <c r="J30" s="151"/>
+      <c r="K30" s="152" t="s">
         <v>161</v>
       </c>
-      <c r="L30" s="185"/>
+      <c r="L30" s="153"/>
     </row>
     <row r="31" spans="1:25" ht="87" customHeight="1">
-      <c r="A31" s="178"/>
-      <c r="B31" s="179"/>
-      <c r="C31" s="179"/>
-      <c r="D31" s="183"/>
-      <c r="E31" s="173">
+      <c r="A31" s="160"/>
+      <c r="B31" s="161"/>
+      <c r="C31" s="161"/>
+      <c r="D31" s="162"/>
+      <c r="E31" s="154">
         <f>(L28/150)</f>
         <v>1.511466666666667</v>
       </c>
-      <c r="F31" s="174"/>
-      <c r="G31" s="175"/>
-      <c r="H31" s="173">
+      <c r="F31" s="155"/>
+      <c r="G31" s="156"/>
+      <c r="H31" s="154">
         <f>(L28^(0.4))</f>
         <v>8.7537861564705111</v>
       </c>
-      <c r="I31" s="174"/>
-      <c r="J31" s="175"/>
-      <c r="K31" s="176">
+      <c r="I31" s="155"/>
+      <c r="J31" s="156"/>
+      <c r="K31" s="129">
         <f>E31*H31</f>
         <v>13.231055982633297</v>
       </c>
-      <c r="L31" s="172" t="s">
+      <c r="L31" s="128" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="87" customHeight="1">
-      <c r="A32" s="180" t="s">
-        <v>164</v>
-      </c>
-      <c r="B32" s="181"/>
-      <c r="C32" s="181"/>
-      <c r="D32" s="182"/>
-      <c r="E32" s="186">
+      <c r="A32" s="146" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="148"/>
+      <c r="E32" s="157">
         <v>4</v>
       </c>
-      <c r="F32" s="187"/>
-      <c r="G32" s="187"/>
-      <c r="H32" s="187"/>
-      <c r="I32" s="187"/>
-      <c r="J32" s="188"/>
-      <c r="K32" s="176">
+      <c r="F32" s="158"/>
+      <c r="G32" s="158"/>
+      <c r="H32" s="158"/>
+      <c r="I32" s="158"/>
+      <c r="J32" s="159"/>
+      <c r="K32" s="129">
         <f>K31/E32</f>
         <v>3.3077639956583242</v>
       </c>
-      <c r="L32" s="172" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="87" hidden="1" customHeight="1">
-      <c r="A33" s="180" t="s">
+      <c r="L32" s="128" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="84" customHeight="1">
+      <c r="A33" s="146" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="147"/>
+      <c r="C33" s="147"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="193" t="s">
+        <v>167</v>
+      </c>
+      <c r="F33" s="194"/>
+      <c r="G33" s="195"/>
+      <c r="H33" s="190">
+        <f>20*K32</f>
+        <v>66.155279913166481</v>
+      </c>
+      <c r="I33" s="191"/>
+      <c r="J33" s="192"/>
+      <c r="K33" s="129">
+        <f>H33*6</f>
+        <v>396.93167947899889</v>
+      </c>
+      <c r="L33" s="128" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="181"/>
-      <c r="C33" s="181"/>
-      <c r="D33" s="182"/>
-      <c r="E33" s="189">
-        <f>2417.9034/390</f>
-        <v>6.1997523076923082</v>
-      </c>
-      <c r="F33" s="190"/>
-      <c r="G33" s="190"/>
-      <c r="H33" s="190"/>
-      <c r="I33" s="190"/>
-      <c r="J33" s="191"/>
-      <c r="K33" s="176"/>
-      <c r="L33" s="172"/>
     </row>
     <row r="34" spans="1:12" ht="20.25">
-      <c r="A34" s="177"/>
-      <c r="B34" s="164"/>
-      <c r="C34" s="164"/>
-      <c r="D34" s="164"/>
-      <c r="E34" s="164"/>
+      <c r="A34" s="130"/>
+      <c r="B34" s="126"/>
+      <c r="C34" s="126"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="126"/>
     </row>
     <row r="35" spans="1:12" ht="20.25">
-      <c r="A35" s="177"/>
-      <c r="B35" s="164"/>
-      <c r="C35" s="164"/>
-      <c r="D35" s="164"/>
-      <c r="E35" s="164"/>
+      <c r="A35" s="130"/>
+      <c r="B35" s="126"/>
+      <c r="C35" s="126"/>
+      <c r="D35" s="126"/>
+      <c r="E35" s="126"/>
     </row>
     <row r="36" spans="1:12" ht="20.25">
-      <c r="A36" s="177"/>
-      <c r="B36" s="164"/>
-      <c r="C36" s="164"/>
-      <c r="D36" s="164"/>
-      <c r="E36" s="164"/>
+      <c r="A36" s="130"/>
+      <c r="B36" s="126"/>
+      <c r="C36" s="126"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="126"/>
     </row>
     <row r="37" spans="1:12" ht="20.25">
-      <c r="A37" s="177"/>
+      <c r="A37" s="130"/>
     </row>
     <row r="38" spans="1:12" ht="24">
-      <c r="A38" s="177"/>
-      <c r="B38" s="192"/>
+      <c r="A38" s="130"/>
+      <c r="B38" s="131"/>
     </row>
     <row r="39" spans="1:12" ht="20.25">
-      <c r="A39" s="177"/>
+      <c r="A39" s="130"/>
     </row>
     <row r="40" spans="1:12" ht="20.25">
-      <c r="A40" s="177"/>
+      <c r="A40" s="130"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="O22:Y23"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O12:Y13"/>
-    <mergeCell ref="O14:Y15"/>
-    <mergeCell ref="O16:Y17"/>
-    <mergeCell ref="O18:Y19"/>
-    <mergeCell ref="O20:Y21"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="B23:K23"/>
-    <mergeCell ref="B24:K24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B17:K17"/>
-    <mergeCell ref="B18:K18"/>
-    <mergeCell ref="B19:K19"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="B22:K22"/>
+  <mergeCells count="58">
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="A8:K8"/>
@@ -44740,6 +44726,48 @@
     <mergeCell ref="B14:K14"/>
     <mergeCell ref="B15:K15"/>
     <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B17:K17"/>
+    <mergeCell ref="B18:K18"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="B20:K20"/>
+    <mergeCell ref="B22:K22"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="O12:Y13"/>
+    <mergeCell ref="O14:Y15"/>
+    <mergeCell ref="O16:Y17"/>
+    <mergeCell ref="O18:Y19"/>
+    <mergeCell ref="O20:Y21"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="O22:Y23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="B23:K23"/>
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="E31:G31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>